<commit_message>
szepseghiba javítások + zip-ek eltavolitasa
</commit_message>
<xml_diff>
--- a/VBJWeboldal/wwwroot/uploads/timetable.xlsx
+++ b/VBJWeboldal/wwwroot/uploads/timetable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Balázs\Iskola\Asp.Net\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF38C11-C0EF-441C-B7F3-5C164A724C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9185E46C-7A81-430D-9CA6-FF6213070FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" activeTab="1" xr2:uid="{06E244FC-3EE1-4C1B-B330-61B9477B0C8C}"/>
   </bookViews>
@@ -1050,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD79E49D-456E-4A59-AA49-4C241270BF3E}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="J100" sqref="J100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.08984375" defaultRowHeight="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2234,22 +2234,22 @@
         <v>57</v>
       </c>
       <c r="B52" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F52" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2263,16 +2263,16 @@
         <v>44</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F53" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2280,22 +2280,22 @@
         <v>57</v>
       </c>
       <c r="B54" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F54" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2309,16 +2309,16 @@
         <v>44</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F55" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2326,22 +2326,22 @@
         <v>57</v>
       </c>
       <c r="B56" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F56" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2355,16 +2355,16 @@
         <v>44</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2372,7 +2372,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>44</v>
@@ -2381,13 +2381,13 @@
         <v>131</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F58" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2401,16 +2401,16 @@
         <v>44</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F59" s="2">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2418,22 +2418,22 @@
         <v>57</v>
       </c>
       <c r="B60" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F60" s="2">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2447,16 +2447,16 @@
         <v>44</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F61" s="2">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2464,22 +2464,22 @@
         <v>57</v>
       </c>
       <c r="B62" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F62" s="2">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2493,39 +2493,39 @@
         <v>44</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F63" s="2">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B64" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F64" s="2">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2539,16 +2539,16 @@
         <v>44</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F65" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2556,22 +2556,22 @@
         <v>79</v>
       </c>
       <c r="B66" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F66" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2585,16 +2585,16 @@
         <v>44</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F67" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2602,22 +2602,22 @@
         <v>79</v>
       </c>
       <c r="B68" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F68" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2631,16 +2631,16 @@
         <v>44</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F69" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2648,22 +2648,22 @@
         <v>79</v>
       </c>
       <c r="B70" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F70" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2671,22 +2671,22 @@
         <v>79</v>
       </c>
       <c r="B71" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F71" s="2">
         <v>21</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2694,7 +2694,7 @@
         <v>79</v>
       </c>
       <c r="B72" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>44</v>
@@ -2717,7 +2717,7 @@
         <v>79</v>
       </c>
       <c r="B73" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>44</v>
@@ -2737,25 +2737,25 @@
     </row>
     <row r="74" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B74" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F74" s="2">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2763,19 +2763,19 @@
         <v>93</v>
       </c>
       <c r="B75" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F75" s="2">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>70</v>
@@ -2786,22 +2786,22 @@
         <v>93</v>
       </c>
       <c r="B76" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F76" s="2">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2815,16 +2815,16 @@
         <v>44</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F77" s="2">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2832,22 +2832,22 @@
         <v>93</v>
       </c>
       <c r="B78" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F78" s="2">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2861,16 +2861,16 @@
         <v>44</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F79" s="2">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2878,22 +2878,22 @@
         <v>93</v>
       </c>
       <c r="B80" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F80" s="2">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2901,22 +2901,22 @@
         <v>93</v>
       </c>
       <c r="B81" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F81" s="2">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2930,16 +2930,16 @@
         <v>44</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="F82" s="2">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2947,22 +2947,22 @@
         <v>93</v>
       </c>
       <c r="B83" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F83" s="2">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2976,24 +2976,24 @@
         <v>44</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="F84" s="2">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B85" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>44</v>
@@ -3008,7 +3008,7 @@
         <v>30</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3022,16 +3022,16 @@
         <v>44</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F86" s="2">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3039,22 +3039,22 @@
         <v>107</v>
       </c>
       <c r="B87" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F87" s="2">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3068,16 +3068,16 @@
         <v>44</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F88" s="2">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3085,22 +3085,22 @@
         <v>107</v>
       </c>
       <c r="B89" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F89" s="2">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3114,16 +3114,16 @@
         <v>44</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F90" s="2">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3131,19 +3131,19 @@
         <v>107</v>
       </c>
       <c r="B91" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="F91" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>118</v>
@@ -3154,7 +3154,7 @@
         <v>107</v>
       </c>
       <c r="B92" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>44</v>
@@ -3174,25 +3174,25 @@
     </row>
     <row r="93" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B93" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="F93" s="2">
         <v>23</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3206,16 +3206,16 @@
         <v>44</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="F94" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>